<commit_message>
Added a prompt for changing the auto refresh rate.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/temp.xlsx
+++ b/src/main/resources/data/temp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <xr:revisionPtr revIDLastSave="53" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36404DF5-C5A1-4552-AFCD-18F3D3A43858}"/>
   <bookViews>
@@ -423,7 +423,7 @@
       </c>
       <c r="C4">
         <f ca="1">C3+RANDBETWEEN(-10,50)</f>
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -433,7 +433,7 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C50" ca="1" si="1">C4+RANDBETWEEN(-10,50)</f>
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -443,7 +443,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>188</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -453,7 +453,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>205</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:3">
@@ -463,7 +463,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>244</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="2:3">
@@ -473,7 +473,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>260</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="2:3">
@@ -483,7 +483,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>264</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="2:3">
@@ -493,7 +493,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -503,7 +503,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>280</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -513,7 +513,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>286</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="2:3">
@@ -523,7 +523,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>292</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="2:3">
@@ -533,7 +533,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>302</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="2:3">
@@ -543,7 +543,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>330</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="2:3">
@@ -553,7 +553,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>344</v>
+        <v>456</v>
       </c>
     </row>
     <row r="18" spans="2:3">
@@ -563,7 +563,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>350</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="2:3">
@@ -573,7 +573,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>383</v>
+        <v>515</v>
       </c>
     </row>
     <row r="20" spans="2:3">
@@ -583,7 +583,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>405</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="2:3">
@@ -593,7 +593,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>411</v>
+        <v>544</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -603,7 +603,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>451</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -613,7 +613,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>458</v>
+        <v>564</v>
       </c>
     </row>
     <row r="24" spans="2:3">
@@ -623,7 +623,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>503</v>
+        <v>601</v>
       </c>
     </row>
     <row r="25" spans="2:3">
@@ -633,7 +633,7 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>551</v>
+        <v>636</v>
       </c>
     </row>
     <row r="26" spans="2:3">
@@ -643,7 +643,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>577</v>
+        <v>636</v>
       </c>
     </row>
     <row r="27" spans="2:3">
@@ -653,7 +653,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>591</v>
+        <v>647</v>
       </c>
     </row>
     <row r="28" spans="2:3">
@@ -663,7 +663,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>600</v>
+        <v>655</v>
       </c>
     </row>
     <row r="29" spans="2:3">
@@ -673,7 +673,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>628</v>
+        <v>661</v>
       </c>
     </row>
     <row r="30" spans="2:3">
@@ -683,7 +683,7 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>649</v>
+        <v>690</v>
       </c>
     </row>
     <row r="31" spans="2:3">
@@ -693,7 +693,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>656</v>
+        <v>721</v>
       </c>
     </row>
     <row r="32" spans="2:3">
@@ -703,7 +703,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>653</v>
+        <v>729</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -713,7 +713,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
-        <v>695</v>
+        <v>773</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -723,7 +723,7 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>715</v>
+        <v>796</v>
       </c>
     </row>
     <row r="35" spans="2:3">
@@ -733,7 +733,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>713</v>
+        <v>814</v>
       </c>
     </row>
     <row r="36" spans="2:3">
@@ -743,7 +743,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="1"/>
-        <v>737</v>
+        <v>811</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -753,7 +753,7 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="1"/>
-        <v>730</v>
+        <v>801</v>
       </c>
     </row>
     <row r="38" spans="2:3">
@@ -763,7 +763,7 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="1"/>
-        <v>735</v>
+        <v>821</v>
       </c>
     </row>
     <row r="39" spans="2:3">
@@ -773,7 +773,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>733</v>
+        <v>846</v>
       </c>
     </row>
     <row r="40" spans="2:3">
@@ -783,7 +783,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>739</v>
+        <v>880</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -793,7 +793,7 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>730</v>
+        <v>905</v>
       </c>
     </row>
     <row r="42" spans="2:3">
@@ -803,7 +803,7 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>730</v>
+        <v>935</v>
       </c>
     </row>
     <row r="43" spans="2:3">
@@ -813,7 +813,7 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
-        <v>736</v>
+        <v>953</v>
       </c>
     </row>
     <row r="44" spans="2:3">
@@ -823,7 +823,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>778</v>
+        <v>980</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -833,7 +833,7 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="1"/>
-        <v>817</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="46" spans="2:3">
@@ -843,7 +843,7 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>839</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="47" spans="2:3">
@@ -853,7 +853,7 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>834</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="48" spans="2:3">
@@ -863,7 +863,7 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>846</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="49" spans="2:3">
@@ -873,7 +873,7 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>842</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="50" spans="2:3">

</xml_diff>